<commit_message>
Parse data from Fall 2013 to Spring 2016
</commit_message>
<xml_diff>
--- a/processed_data/_2015-2016.xlsx
+++ b/processed_data/_2015-2016.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1520" yWindow="1520" windowWidth="23200" windowHeight="13750" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1890" yWindow="720" windowWidth="22400" windowHeight="13850" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summer 2015" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,19 +19,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -402,8 +395,8 @@
   </sheetPr>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -599,7 +592,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>TCHR LIVES  ENV</t>
+          <t>TCHR LIVES &amp;POL ENV</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -665,7 +658,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TCHR LIVES  ENV</t>
+          <t>TCHR LIVES &amp;POL ENV</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -731,7 +724,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>TCHR LIVES  ENV</t>
+          <t>TCHR LIVES &amp;POL ENV</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -797,7 +790,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>TCHR LIVES  ENV</t>
+          <t>TCHR LIVES &amp;POL ENV</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1127,7 +1120,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ADV CON LEARN</t>
+          <t>ADV CON LEARN&amp;COGNT</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1193,7 +1186,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ADV CON LEARN</t>
+          <t>ADV CON LEARN&amp;COGNT</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1259,7 +1252,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ADV CON LEARN</t>
+          <t>ADV CON LEARN&amp;COGNT</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1325,7 +1318,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ADV CON LEARN</t>
+          <t>ADV CON LEARN&amp;COGNT</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1919,7 +1912,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>INSTRUC DESN  TECH</t>
+          <t>INSTRUC DESN &amp; TECH</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1985,7 +1978,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>INSTRUC DESN  TECH</t>
+          <t>INSTRUC DESN &amp; TECH</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2051,7 +2044,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>INSTRUC DESN  TECH</t>
+          <t>INSTRUC DESN &amp; TECH</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2117,7 +2110,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>INSTRUC DESN  TECH</t>
+          <t>INSTRUC DESN &amp; TECH</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2579,7 +2572,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>IDEOLOGS  ECOLOGS</t>
+          <t>IDEOLOGS &amp; ECOLOGS</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -3819,8 +3812,8 @@
   </sheetPr>
   <dimension ref="A1:P290"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -10350,7 +10343,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>ED POLICY &amp; POLITICS</t>
+          <t>ED POLICY &amp;POLITICS</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -13848,7 +13841,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>FE:BUS &amp; GOVT</t>
+          <t>FE:BUS &amp;GOVT</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -23008,8 +23001,8 @@
   </sheetPr>
   <dimension ref="A1:P263"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G210" sqref="G210"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -26766,7 +26759,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>CRIME &amp; SOC DEVIANCE</t>
+          <t>CRIME &amp;SOC DEVIANCE</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -27294,7 +27287,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>DEV &amp; CELL JRNL CLUB</t>
+          <t>DEV &amp;CELL JRNL CLUB</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -31386,7 +31379,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>FE:BUS &amp; GOVT</t>
+          <t>FE:BUS &amp;GOVT</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -32376,7 +32369,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>DATA &amp; PRGRM ANLYTCS</t>
+          <t>DATA &amp;PRGRM ANLYTCS</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -38052,7 +38045,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>POVERTY &amp; DEVELOPMNT</t>
+          <t>POVERTY &amp;DEVELOPMNT</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -40414,8 +40407,8 @@
   </sheetPr>
   <dimension ref="A1:P240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:P1"/>
+    <sheetView topLeftCell="A193" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q234" sqref="Q234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -43381,7 +43374,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>MDWR NTWK &amp; DIST SYS</t>
+          <t>MDWR NTWK &amp;DIST SYS</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -46879,7 +46872,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>MICRO-SENS &amp; ACTUATR</t>
+          <t>MICRO-SENS&amp; ACTUATR</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -55987,7 +55980,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>GLOBAL &amp; DEMG CHANGE</t>
+          <t>GLOBAL&amp; DEMG CHANGE</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">

</xml_diff>